<commit_message>
Add match count; add float row/col output in LocationListing.csv
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/LocatorListing.xlsx
+++ b/Assets/StreamingAssets/LocatorListing.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Projects\GitHub\FaceCards\Assets\StreamingAssets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalvarado\Documents\GitHub\FaceCards\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23460" windowHeight="14100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23460" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocatorListing" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LocatorListing!$A$1:$D$136</definedName>
+  </definedNames>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -442,7 +445,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1298,19 +1301,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" hidden="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1327,2033 +1325,2034 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>9</v>
       </c>
-      <c r="C2" s="1">
-        <v>24</v>
+      <c r="C2">
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B2-1)&amp;" "&amp;C2</f>
-        <v>I 24</v>
+        <v>I 20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
-        <v>28</v>
+      <c r="C3">
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B3-1)&amp;" "&amp;C3</f>
-        <v>I 28</v>
+        <v>I 24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
-        <v>25</v>
+      <c r="C4">
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B4-1)&amp;" "&amp;C4</f>
-        <v>B 25</v>
+        <v>B 21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>24</v>
       </c>
-      <c r="C5" s="1">
-        <v>22</v>
+      <c r="C5">
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B5-1)&amp;" "&amp;C5</f>
-        <v>X 22</v>
+        <v>X 18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>14</v>
       </c>
-      <c r="C6" s="1">
-        <v>16</v>
+      <c r="C6">
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B6-1)&amp;" "&amp;C6</f>
-        <v>N 16</v>
+        <v>N 12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
-        <v>23</v>
+      <c r="C7">
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B7-1)&amp;" "&amp;C7</f>
-        <v>G 23</v>
+        <v>G 20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>14</v>
       </c>
-      <c r="C8" s="1">
-        <v>12</v>
+      <c r="C8">
+        <v>8</v>
       </c>
       <c r="D8" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B8-1)&amp;" "&amp;C8</f>
-        <v>N 12</v>
+        <v>N 8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
-        <v>19</v>
+      <c r="C9">
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B9-1)&amp;" "&amp;C9</f>
-        <v>G 19</v>
+        <v>G 15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10" s="1">
-        <v>11</v>
+      <c r="C10">
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B10-1)&amp;" "&amp;C10</f>
-        <v>C 11</v>
+        <v>C 7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>25</v>
       </c>
-      <c r="C11" s="1">
-        <v>29</v>
+      <c r="C11">
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B11-1)&amp;" "&amp;C11</f>
-        <v>Y 29</v>
+        <v>Y 26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>133</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>5</v>
       </c>
-      <c r="C12" s="1">
-        <v>10</v>
+      <c r="C12">
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B12-1)&amp;" "&amp;C12</f>
-        <v>E 10</v>
+        <v>E 6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>18</v>
       </c>
-      <c r="C13" s="1">
-        <v>26</v>
+      <c r="C13">
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B13-1)&amp;" "&amp;C13</f>
-        <v>R 26</v>
+        <v>R 22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>3</v>
       </c>
-      <c r="C14" s="1">
-        <v>20</v>
+      <c r="C14">
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B14-1)&amp;" "&amp;C14</f>
-        <v>C 20</v>
+        <v>C 16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>19</v>
       </c>
-      <c r="C15" s="1">
-        <v>24</v>
+      <c r="C15">
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B15-1)&amp;" "&amp;C15</f>
-        <v>S 24</v>
+        <v>S 20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>10</v>
       </c>
-      <c r="C16" s="1">
-        <v>28</v>
+      <c r="C16">
+        <v>24</v>
       </c>
       <c r="D16" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B16-1)&amp;" "&amp;C16</f>
-        <v>J 28</v>
+        <v>J 24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>19</v>
       </c>
-      <c r="C17" s="1">
-        <v>20</v>
+      <c r="C17">
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B17-1)&amp;" "&amp;C17</f>
-        <v>S 20</v>
+        <v>S 16</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>14</v>
       </c>
-      <c r="C18" s="1">
-        <v>20</v>
+      <c r="C18">
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B18-1)&amp;" "&amp;C18</f>
-        <v>N 20</v>
+        <v>N 16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>9</v>
       </c>
-      <c r="C19" s="1">
-        <v>20</v>
+      <c r="C19">
+        <v>16</v>
       </c>
       <c r="D19" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B19-1)&amp;" "&amp;C19</f>
-        <v>I 20</v>
+        <v>I 16</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20">
         <v>20</v>
       </c>
-      <c r="C20" s="1">
-        <v>34</v>
+      <c r="C20">
+        <v>30</v>
       </c>
       <c r="D20" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B20-1)&amp;" "&amp;C20</f>
-        <v>T 34</v>
+        <v>T 30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21">
         <v>17</v>
       </c>
-      <c r="C21" s="1">
-        <v>25</v>
+      <c r="C21">
+        <v>21</v>
       </c>
       <c r="D21" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B21-1)&amp;" "&amp;C21</f>
-        <v>Q 25</v>
+        <v>Q 21</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>17</v>
       </c>
-      <c r="C22" s="1">
-        <v>32</v>
+      <c r="C22">
+        <v>28</v>
       </c>
       <c r="D22" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B22-1)&amp;" "&amp;C22</f>
-        <v>Q 32</v>
+        <v>Q 28</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
         <v>11</v>
       </c>
-      <c r="C23" s="1">
-        <v>19</v>
+      <c r="C23">
+        <v>15</v>
       </c>
       <c r="D23" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B23-1)&amp;" "&amp;C23</f>
-        <v>K 19</v>
+        <v>K 15</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24">
         <v>15</v>
       </c>
-      <c r="C24" s="1">
-        <v>14</v>
+      <c r="C24">
+        <v>10</v>
       </c>
       <c r="D24" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B24-1)&amp;" "&amp;C24</f>
-        <v>O 14</v>
+        <v>O 10</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
         <v>13</v>
       </c>
-      <c r="C25" s="1">
-        <v>14</v>
+      <c r="C25">
+        <v>10</v>
       </c>
       <c r="D25" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B25-1)&amp;" "&amp;C25</f>
-        <v>M 14</v>
+        <v>M 10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26">
         <v>5</v>
       </c>
-      <c r="C26" s="1">
-        <v>9</v>
+      <c r="C26">
+        <v>5</v>
       </c>
       <c r="D26" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B26-1)&amp;" "&amp;C26</f>
-        <v>E 9</v>
+        <v>E 5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
         <v>17</v>
       </c>
-      <c r="C27" s="1">
-        <v>33</v>
+      <c r="C27">
+        <v>29</v>
       </c>
       <c r="D27" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B27-1)&amp;" "&amp;C27</f>
-        <v>Q 33</v>
+        <v>Q 29</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28">
         <v>10</v>
       </c>
-      <c r="C28" s="1">
-        <v>22</v>
+      <c r="C28">
+        <v>18</v>
       </c>
       <c r="D28" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B28-1)&amp;" "&amp;C28</f>
-        <v>J 22</v>
+        <v>J 18</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29">
         <v>4</v>
       </c>
-      <c r="C29" s="1">
-        <v>28</v>
+      <c r="C29">
+        <v>24</v>
       </c>
       <c r="D29" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B29-1)&amp;" "&amp;C29</f>
-        <v>D 28</v>
+        <v>D 24</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30">
         <v>21</v>
       </c>
-      <c r="C30" s="1">
-        <v>29</v>
+      <c r="C30">
+        <v>25</v>
       </c>
       <c r="D30" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B30-1)&amp;" "&amp;C30</f>
-        <v>U 29</v>
+        <v>U 25</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31">
         <v>8</v>
       </c>
-      <c r="C31" s="1">
-        <v>28</v>
+      <c r="C31">
+        <v>25</v>
       </c>
       <c r="D31" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B31-1)&amp;" "&amp;C31</f>
-        <v>H 28</v>
+        <v>H 25</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32">
         <v>13</v>
       </c>
-      <c r="C32" s="1">
-        <v>18</v>
+      <c r="C32">
+        <v>14</v>
       </c>
       <c r="D32" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B32-1)&amp;" "&amp;C32</f>
-        <v>M 18</v>
+        <v>M 14</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>106</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33" s="1">
-        <v>29</v>
+      <c r="C33">
+        <v>25</v>
       </c>
       <c r="D33" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B33-1)&amp;" "&amp;C33</f>
-        <v>A 29</v>
+        <v>A 25</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34">
         <v>15</v>
       </c>
-      <c r="C34" s="1">
-        <v>7</v>
+      <c r="C34">
+        <v>3</v>
       </c>
       <c r="D34" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B34-1)&amp;" "&amp;C34</f>
-        <v>O 7</v>
+        <v>O 3</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>128</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35">
         <v>8</v>
       </c>
-      <c r="C35" s="1">
-        <v>23</v>
+      <c r="C35">
+        <v>19</v>
       </c>
       <c r="D35" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B35-1)&amp;" "&amp;C35</f>
-        <v>H 23</v>
+        <v>H 19</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36">
         <v>8</v>
       </c>
-      <c r="C36" s="1">
-        <v>34</v>
+      <c r="C36">
+        <v>30</v>
       </c>
       <c r="D36" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B36-1)&amp;" "&amp;C36</f>
-        <v>H 34</v>
+        <v>H 30</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>135</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37">
         <v>3</v>
       </c>
-      <c r="C37" s="1">
-        <v>9</v>
+      <c r="C37">
+        <v>5</v>
       </c>
       <c r="D37" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B37-1)&amp;" "&amp;C37</f>
-        <v>C 9</v>
+        <v>C 5</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>117</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38">
         <v>6</v>
       </c>
-      <c r="C38" s="1">
-        <v>21</v>
+      <c r="C38">
+        <v>17</v>
       </c>
       <c r="D38" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B38-1)&amp;" "&amp;C38</f>
-        <v>F 21</v>
+        <v>F 17</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39">
         <v>15</v>
       </c>
-      <c r="C39" s="1">
-        <v>26</v>
+      <c r="C39">
+        <v>22</v>
       </c>
       <c r="D39" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B39-1)&amp;" "&amp;C39</f>
-        <v>O 26</v>
+        <v>O 22</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40">
         <v>19</v>
       </c>
-      <c r="C40" s="1">
-        <v>29</v>
+      <c r="C40">
+        <v>25</v>
       </c>
       <c r="D40" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B40-1)&amp;" "&amp;C40</f>
-        <v>S 29</v>
+        <v>S 25</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>131</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41">
         <v>14</v>
       </c>
-      <c r="C41" s="1">
-        <v>40</v>
+      <c r="C41">
+        <v>36</v>
       </c>
       <c r="D41" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B41-1)&amp;" "&amp;C41</f>
-        <v>N 40</v>
+        <v>N 36</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>132</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42">
         <v>13</v>
       </c>
-      <c r="C42" s="1">
-        <v>26</v>
+      <c r="C42">
+        <v>23</v>
       </c>
       <c r="D42" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B42-1)&amp;" "&amp;C42</f>
-        <v>M 26</v>
+        <v>M 23</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43">
         <v>18</v>
       </c>
-      <c r="C43" s="1">
-        <v>30</v>
+      <c r="C43">
+        <v>27</v>
       </c>
       <c r="D43" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B43-1)&amp;" "&amp;C43</f>
-        <v>R 30</v>
+        <v>R 27</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44">
         <v>8</v>
       </c>
-      <c r="C44" s="1">
-        <v>7</v>
+      <c r="C44">
+        <v>3</v>
       </c>
       <c r="D44" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B44-1)&amp;" "&amp;C44</f>
-        <v>H 7</v>
+        <v>H 3</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45">
         <v>9</v>
       </c>
-      <c r="C45" s="1">
-        <v>31</v>
+      <c r="C45">
+        <v>27</v>
       </c>
       <c r="D45" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B45-1)&amp;" "&amp;C45</f>
-        <v>I 31</v>
+        <v>I 27</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46">
         <v>14</v>
       </c>
-      <c r="C46" s="1">
-        <v>16</v>
+      <c r="C46">
+        <v>12</v>
       </c>
       <c r="D46" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B46-1)&amp;" "&amp;C46</f>
-        <v>N 16</v>
+        <v>N 12</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="1">
-        <v>26</v>
-      </c>
-      <c r="C47" s="1">
+      <c r="B47">
         <v>25</v>
+      </c>
+      <c r="C47">
+        <v>21</v>
       </c>
       <c r="D47" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B47-1)&amp;" "&amp;C47</f>
-        <v>Z 25</v>
+        <v>Y 21</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>10</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48">
         <v>21</v>
       </c>
-      <c r="C48" s="1">
-        <v>40</v>
+      <c r="C48">
+        <v>36</v>
       </c>
       <c r="D48" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B48-1)&amp;" "&amp;C48</f>
-        <v>U 40</v>
+        <v>U 36</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>34</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49">
         <v>13</v>
       </c>
-      <c r="C49" s="1">
-        <v>10</v>
+      <c r="C49">
+        <v>6</v>
       </c>
       <c r="D49" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B49-1)&amp;" "&amp;C49</f>
-        <v>M 10</v>
+        <v>M 6</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="1">
-        <v>26</v>
-      </c>
-      <c r="C50" s="1">
-        <v>31</v>
+      <c r="B50">
+        <v>25</v>
+      </c>
+      <c r="C50">
+        <v>27</v>
       </c>
       <c r="D50" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B50-1)&amp;" "&amp;C50</f>
-        <v>Z 31</v>
+        <v>Y 27</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>73</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51">
         <v>6</v>
       </c>
-      <c r="C51" s="1">
-        <v>15</v>
+      <c r="C51">
+        <v>11</v>
       </c>
       <c r="D51" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B51-1)&amp;" "&amp;C51</f>
-        <v>F 15</v>
+        <v>F 11</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>69</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52">
         <v>2</v>
       </c>
-      <c r="C52" s="1">
-        <v>27</v>
+      <c r="C52">
+        <v>23</v>
       </c>
       <c r="D52" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B52-1)&amp;" "&amp;C52</f>
-        <v>B 27</v>
+        <v>B 23</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>115</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53">
         <v>17</v>
       </c>
-      <c r="C53" s="1">
-        <v>29</v>
+      <c r="C53">
+        <v>25</v>
       </c>
       <c r="D53" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B53-1)&amp;" "&amp;C53</f>
-        <v>Q 29</v>
+        <v>Q 25</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54">
         <v>21</v>
       </c>
-      <c r="C54" s="1">
-        <v>32</v>
+      <c r="C54">
+        <v>28</v>
       </c>
       <c r="D54" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B54-1)&amp;" "&amp;C54</f>
-        <v>U 32</v>
+        <v>U 28</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55">
         <v>14</v>
       </c>
-      <c r="C55" s="1">
-        <v>24</v>
+      <c r="C55">
+        <v>20</v>
       </c>
       <c r="D55" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B55-1)&amp;" "&amp;C55</f>
-        <v>N 24</v>
+        <v>N 20</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>126</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56">
         <v>14</v>
       </c>
-      <c r="C56" s="1">
-        <v>20</v>
+      <c r="C56">
+        <v>16</v>
       </c>
       <c r="D56" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B56-1)&amp;" "&amp;C56</f>
-        <v>N 20</v>
+        <v>N 16</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>49</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57">
         <v>8</v>
       </c>
-      <c r="C57" s="1">
-        <v>33</v>
+      <c r="C57">
+        <v>29</v>
       </c>
       <c r="D57" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B57-1)&amp;" "&amp;C57</f>
-        <v>H 33</v>
+        <v>H 29</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58">
         <v>7</v>
       </c>
-      <c r="C58" s="1">
-        <v>24</v>
+      <c r="C58">
+        <v>20</v>
       </c>
       <c r="D58" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B58-1)&amp;" "&amp;C58</f>
-        <v>G 24</v>
+        <v>G 20</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>39</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59">
         <v>13</v>
       </c>
-      <c r="C59" s="1">
-        <v>14</v>
+      <c r="C59">
+        <v>10</v>
       </c>
       <c r="D59" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B59-1)&amp;" "&amp;C59</f>
-        <v>M 14</v>
+        <v>M 10</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="A60" t="s">
         <v>87</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60">
         <v>2</v>
       </c>
-      <c r="C60" s="1">
-        <v>11</v>
+      <c r="C60">
+        <v>7</v>
       </c>
       <c r="D60" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B60-1)&amp;" "&amp;C60</f>
-        <v>B 11</v>
+        <v>B 7</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>119</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61">
         <v>3</v>
       </c>
-      <c r="C61" s="1">
-        <v>15</v>
+      <c r="C61">
+        <v>11</v>
       </c>
       <c r="D61" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B61-1)&amp;" "&amp;C61</f>
-        <v>C 15</v>
+        <v>C 11</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>96</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62">
         <v>21</v>
       </c>
-      <c r="C62" s="1">
-        <v>28</v>
+      <c r="C62">
+        <v>24</v>
       </c>
       <c r="D62" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B62-1)&amp;" "&amp;C62</f>
-        <v>U 28</v>
+        <v>U 24</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>80</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63">
         <v>6</v>
       </c>
-      <c r="C63" s="1">
-        <v>34</v>
+      <c r="C63">
+        <v>30</v>
       </c>
       <c r="D63" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B63-1)&amp;" "&amp;C63</f>
-        <v>F 34</v>
+        <v>F 30</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>47</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64">
         <v>19</v>
       </c>
-      <c r="C64" s="1">
-        <v>21</v>
+      <c r="C64">
+        <v>17</v>
       </c>
       <c r="D64" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B64-1)&amp;" "&amp;C64</f>
-        <v>S 21</v>
+        <v>S 17</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>35</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65">
         <v>4</v>
       </c>
-      <c r="C65" s="1">
-        <v>9</v>
+      <c r="C65">
+        <v>5</v>
       </c>
       <c r="D65" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B65-1)&amp;" "&amp;C65</f>
-        <v>D 9</v>
+        <v>D 5</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>137</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66">
         <v>17</v>
       </c>
-      <c r="C66" s="1">
-        <v>24</v>
+      <c r="C66">
+        <v>20</v>
       </c>
       <c r="D66" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B66-1)&amp;" "&amp;C66</f>
-        <v>Q 24</v>
+        <v>Q 20</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="A67" t="s">
         <v>100</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67">
         <v>25</v>
       </c>
-      <c r="C67" s="1">
-        <v>37</v>
+      <c r="C67">
+        <v>33</v>
       </c>
       <c r="D67" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B67-1)&amp;" "&amp;C67</f>
-        <v>Y 37</v>
+        <v>Y 33</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="A68" t="s">
         <v>94</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68">
         <v>5</v>
       </c>
-      <c r="C68" s="1">
-        <v>16</v>
+      <c r="C68">
+        <v>12</v>
       </c>
       <c r="D68" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B68-1)&amp;" "&amp;C68</f>
-        <v>E 16</v>
+        <v>E 12</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="A69" t="s">
         <v>74</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69">
         <v>17</v>
       </c>
-      <c r="C69" s="1">
-        <v>21</v>
+      <c r="C69">
+        <v>17</v>
       </c>
       <c r="D69" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B69-1)&amp;" "&amp;C69</f>
-        <v>Q 21</v>
+        <v>Q 17</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>129</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70">
         <v>10</v>
       </c>
-      <c r="C70" s="1">
-        <v>7</v>
+      <c r="C70">
+        <v>3</v>
       </c>
       <c r="D70" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B70-1)&amp;" "&amp;C70</f>
-        <v>J 7</v>
+        <v>J 3</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="A71" t="s">
         <v>67</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71">
         <v>19</v>
       </c>
-      <c r="C71" s="1">
-        <v>36</v>
+      <c r="C71">
+        <v>32</v>
       </c>
       <c r="D71" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B71-1)&amp;" "&amp;C71</f>
-        <v>S 36</v>
+        <v>S 32</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="A72" t="s">
         <v>123</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72">
         <v>19</v>
       </c>
-      <c r="C72" s="1">
-        <v>32</v>
+      <c r="C72">
+        <v>28</v>
       </c>
       <c r="D72" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B72-1)&amp;" "&amp;C72</f>
-        <v>S 32</v>
+        <v>S 28</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="A73" t="s">
         <v>99</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73">
         <v>15</v>
       </c>
-      <c r="C73" s="1">
-        <v>18</v>
+      <c r="C73">
+        <v>14</v>
       </c>
       <c r="D73" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B73-1)&amp;" "&amp;C73</f>
-        <v>O 18</v>
+        <v>O 14</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
         <v>26</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74">
         <v>5</v>
       </c>
-      <c r="C74" s="1">
-        <v>16</v>
+      <c r="C74">
+        <v>12</v>
       </c>
       <c r="D74" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B74-1)&amp;" "&amp;C74</f>
-        <v>E 16</v>
+        <v>E 12</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="A75" t="s">
         <v>25</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75">
         <v>20</v>
       </c>
-      <c r="C75" s="1">
-        <v>40</v>
+      <c r="C75">
+        <v>36</v>
       </c>
       <c r="D75" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B75-1)&amp;" "&amp;C75</f>
-        <v>T 40</v>
+        <v>T 36</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+      <c r="A76" t="s">
         <v>91</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76">
         <v>7</v>
       </c>
-      <c r="C76" s="1">
-        <v>22</v>
+      <c r="C76">
+        <v>18</v>
       </c>
       <c r="D76" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B76-1)&amp;" "&amp;C76</f>
-        <v>G 22</v>
+        <v>G 18</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="A77" t="s">
         <v>63</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77">
         <v>14</v>
       </c>
-      <c r="C77" s="1">
-        <v>36</v>
+      <c r="C77">
+        <v>32</v>
       </c>
       <c r="D77" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B77-1)&amp;" "&amp;C77</f>
-        <v>N 36</v>
+        <v>N 32</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+      <c r="A78" t="s">
         <v>120</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78">
         <v>3</v>
       </c>
-      <c r="C78" s="1">
-        <v>14</v>
+      <c r="C78">
+        <v>10</v>
       </c>
       <c r="D78" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B78-1)&amp;" "&amp;C78</f>
-        <v>C 14</v>
+        <v>C 10</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="A79" t="s">
         <v>109</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79">
         <v>14</v>
       </c>
-      <c r="C79" s="1">
-        <v>8</v>
+      <c r="C79">
+        <v>4</v>
       </c>
       <c r="D79" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B79-1)&amp;" "&amp;C79</f>
-        <v>N 8</v>
+        <v>N 4</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="A80" t="s">
         <v>118</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80">
         <v>3</v>
       </c>
-      <c r="C80" s="1">
-        <v>10</v>
+      <c r="C80">
+        <v>6</v>
       </c>
       <c r="D80" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B80-1)&amp;" "&amp;C80</f>
-        <v>C 10</v>
+        <v>C 6</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="A81" t="s">
         <v>9</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81">
         <v>20</v>
       </c>
-      <c r="C81" s="1">
-        <v>30</v>
+      <c r="C81">
+        <v>26</v>
       </c>
       <c r="D81" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B81-1)&amp;" "&amp;C81</f>
-        <v>T 30</v>
+        <v>T 26</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="A82" t="s">
         <v>56</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82">
         <v>19</v>
       </c>
-      <c r="C82" s="1">
-        <v>33</v>
+      <c r="C82">
+        <v>29</v>
       </c>
       <c r="D82" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B82-1)&amp;" "&amp;C82</f>
-        <v>S 33</v>
+        <v>S 29</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="A83" t="s">
         <v>28</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83">
         <v>14</v>
       </c>
-      <c r="C83" s="1">
-        <v>24</v>
+      <c r="C83">
+        <v>20</v>
       </c>
       <c r="D83" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B83-1)&amp;" "&amp;C83</f>
-        <v>N 24</v>
+        <v>N 20</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="A84" t="s">
         <v>54</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84">
         <v>15</v>
       </c>
-      <c r="C84" s="1">
-        <v>13</v>
+      <c r="C84">
+        <v>10</v>
       </c>
       <c r="D84" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B84-1)&amp;" "&amp;C84</f>
-        <v>O 13</v>
+        <v>O 10</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="A85" t="s">
         <v>102</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85">
         <v>26</v>
       </c>
-      <c r="C85" s="1">
-        <v>27</v>
+      <c r="C85">
+        <v>23</v>
       </c>
       <c r="D85" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B85-1)&amp;" "&amp;C85</f>
-        <v>Z 27</v>
+        <v>Z 23</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="A86" t="s">
         <v>32</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86">
         <v>15</v>
       </c>
-      <c r="C86" s="1">
-        <v>38</v>
+      <c r="C86">
+        <v>34</v>
       </c>
       <c r="D86" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B86-1)&amp;" "&amp;C86</f>
-        <v>O 38</v>
+        <v>O 34</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="A87" t="s">
         <v>12</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87">
         <v>13</v>
       </c>
-      <c r="C87" s="1">
-        <v>23</v>
+      <c r="C87">
+        <v>19</v>
       </c>
       <c r="D87" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B87-1)&amp;" "&amp;C87</f>
-        <v>M 23</v>
+        <v>M 19</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="A88" t="s">
         <v>51</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88">
         <v>26</v>
       </c>
-      <c r="C88" s="1">
-        <v>33</v>
+      <c r="C88">
+        <v>29</v>
       </c>
       <c r="D88" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B88-1)&amp;" "&amp;C88</f>
-        <v>Z 33</v>
+        <v>Z 29</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="A89" t="s">
         <v>116</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89">
         <v>17</v>
       </c>
-      <c r="C89" s="1">
-        <v>39</v>
+      <c r="C89">
+        <v>35</v>
       </c>
       <c r="D89" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B89-1)&amp;" "&amp;C89</f>
-        <v>Q 39</v>
+        <v>Q 35</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="A90" t="s">
         <v>45</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90">
         <v>2</v>
       </c>
-      <c r="C90" s="1">
-        <v>13</v>
+      <c r="C90">
+        <v>9</v>
       </c>
       <c r="D90" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B90-1)&amp;" "&amp;C90</f>
-        <v>B 13</v>
+        <v>B 9</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="A91" t="s">
         <v>18</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91">
         <v>10</v>
       </c>
-      <c r="C91" s="1">
-        <v>20</v>
+      <c r="C91">
+        <v>16</v>
       </c>
       <c r="D91" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B91-1)&amp;" "&amp;C91</f>
-        <v>J 20</v>
+        <v>J 16</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="A92" t="s">
         <v>136</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92">
         <v>5</v>
       </c>
-      <c r="C92" s="1">
-        <v>12</v>
+      <c r="C92">
+        <v>8</v>
       </c>
       <c r="D92" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B92-1)&amp;" "&amp;C92</f>
-        <v>E 12</v>
+        <v>E 8</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="A93" t="s">
         <v>42</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93">
         <v>13</v>
       </c>
-      <c r="C93" s="1">
-        <v>30</v>
+      <c r="C93">
+        <v>26</v>
       </c>
       <c r="D93" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B93-1)&amp;" "&amp;C93</f>
-        <v>M 30</v>
+        <v>M 26</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="A94" t="s">
         <v>70</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94">
         <v>21</v>
       </c>
-      <c r="C94" s="1">
-        <v>33</v>
+      <c r="C94">
+        <v>29</v>
       </c>
       <c r="D94" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B94-1)&amp;" "&amp;C94</f>
-        <v>U 33</v>
+        <v>U 29</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="A95" t="s">
         <v>55</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95">
         <v>8</v>
       </c>
-      <c r="C95" s="1">
-        <v>20</v>
+      <c r="C95">
+        <v>16</v>
       </c>
       <c r="D95" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B95-1)&amp;" "&amp;C95</f>
-        <v>H 20</v>
+        <v>H 16</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="A96" t="s">
         <v>36</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96">
         <v>21</v>
       </c>
-      <c r="C96" s="1">
-        <v>25</v>
+      <c r="C96">
+        <v>21</v>
       </c>
       <c r="D96" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B96-1)&amp;" "&amp;C96</f>
-        <v>U 25</v>
+        <v>U 21</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+      <c r="A97" t="s">
         <v>85</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97">
         <v>13</v>
       </c>
-      <c r="C97" s="1">
-        <v>7</v>
+      <c r="C97">
+        <v>3</v>
       </c>
       <c r="D97" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B97-1)&amp;" "&amp;C97</f>
-        <v>M 7</v>
+        <v>M 3</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="A98" t="s">
         <v>15</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98">
         <v>13</v>
       </c>
-      <c r="C98" s="1">
-        <v>22</v>
+      <c r="C98">
+        <v>18</v>
       </c>
       <c r="D98" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B98-1)&amp;" "&amp;C98</f>
-        <v>M 22</v>
+        <v>M 18</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="A99" t="s">
         <v>105</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99">
         <v>3</v>
       </c>
-      <c r="C99" s="1">
-        <v>23</v>
+      <c r="C99">
+        <v>19</v>
       </c>
       <c r="D99" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B99-1)&amp;" "&amp;C99</f>
-        <v>C 23</v>
+        <v>C 19</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="A100" t="s">
         <v>78</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100">
         <v>13</v>
       </c>
-      <c r="C100" s="1">
-        <v>8</v>
+      <c r="C100">
+        <v>4</v>
       </c>
       <c r="D100" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B100-1)&amp;" "&amp;C100</f>
-        <v>M 8</v>
+        <v>M 4</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="A101" t="s">
         <v>50</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101">
         <v>17</v>
       </c>
-      <c r="C101" s="1">
-        <v>20</v>
+      <c r="C101">
+        <v>16</v>
       </c>
       <c r="D101" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B101-1)&amp;" "&amp;C101</f>
-        <v>Q 20</v>
+        <v>Q 16</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="A102" t="s">
         <v>24</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102">
         <v>2</v>
       </c>
-      <c r="C102" s="1">
-        <v>15</v>
+      <c r="C102">
+        <v>12</v>
       </c>
       <c r="D102" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B102-1)&amp;" "&amp;C102</f>
-        <v>B 15</v>
+        <v>B 12</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+      <c r="A103" t="s">
         <v>134</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103">
         <v>18</v>
       </c>
-      <c r="C103" s="1">
-        <v>22</v>
+      <c r="C103">
+        <v>18</v>
       </c>
       <c r="D103" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B103-1)&amp;" "&amp;C103</f>
-        <v>R 22</v>
+        <v>R 18</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="A104" t="s">
         <v>98</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104">
         <v>9</v>
       </c>
-      <c r="C104" s="1">
-        <v>6</v>
+      <c r="C104">
+        <v>2</v>
       </c>
       <c r="D104" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B104-1)&amp;" "&amp;C104</f>
-        <v>I 6</v>
+        <v>I 2</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+      <c r="A105" t="s">
         <v>16</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105">
         <v>5</v>
       </c>
-      <c r="C105" s="1">
-        <v>11</v>
+      <c r="C105">
+        <v>7</v>
       </c>
       <c r="D105" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B105-1)&amp;" "&amp;C105</f>
-        <v>E 11</v>
+        <v>E 7</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+      <c r="A106" t="s">
         <v>86</v>
       </c>
-      <c r="B106" s="1">
-        <v>21</v>
-      </c>
-      <c r="C106" s="1">
-        <v>14</v>
+      <c r="B106">
+        <v>20</v>
+      </c>
+      <c r="C106">
+        <v>4</v>
       </c>
       <c r="D106" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B106-1)&amp;" "&amp;C106</f>
-        <v>U 14</v>
+        <v>T 4</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+      <c r="A107" t="s">
         <v>19</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107">
         <v>18</v>
       </c>
-      <c r="C107" s="1">
-        <v>40</v>
+      <c r="C107">
+        <v>36</v>
       </c>
       <c r="D107" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B107-1)&amp;" "&amp;C107</f>
-        <v>R 40</v>
+        <v>R 36</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="A108" t="s">
         <v>72</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108">
         <v>7</v>
       </c>
-      <c r="C108" s="1">
-        <v>29</v>
+      <c r="C108">
+        <v>25</v>
       </c>
       <c r="D108" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B108-1)&amp;" "&amp;C108</f>
-        <v>G 29</v>
+        <v>G 25</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="A109" t="s">
         <v>76</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109">
         <v>15</v>
       </c>
-      <c r="C109" s="1">
-        <v>8</v>
+      <c r="C109">
+        <v>4</v>
       </c>
       <c r="D109" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B109-1)&amp;" "&amp;C109</f>
-        <v>O 8</v>
+        <v>O 4</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="A110" t="s">
         <v>31</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110">
         <v>13</v>
       </c>
-      <c r="C110" s="1">
-        <v>30</v>
+      <c r="C110">
+        <v>27</v>
       </c>
       <c r="D110" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B110-1)&amp;" "&amp;C110</f>
-        <v>M 30</v>
+        <v>M 27</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="A111" t="s">
         <v>11</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B111">
         <v>10</v>
       </c>
-      <c r="C111" s="1">
-        <v>23</v>
+      <c r="C111">
+        <v>19</v>
       </c>
       <c r="D111" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B111-1)&amp;" "&amp;C111</f>
-        <v>J 23</v>
+        <v>J 19</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+      <c r="A112" t="s">
         <v>89</v>
       </c>
-      <c r="B112" s="1">
+      <c r="B112">
         <v>21</v>
       </c>
-      <c r="C112" s="1">
-        <v>24</v>
+      <c r="C112">
+        <v>20</v>
       </c>
       <c r="D112" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B112-1)&amp;" "&amp;C112</f>
-        <v>U 24</v>
+        <v>U 20</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+      <c r="A113" t="s">
         <v>58</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113">
         <v>6</v>
       </c>
-      <c r="C113" s="1">
-        <v>13</v>
+      <c r="C113">
+        <v>9</v>
       </c>
       <c r="D113" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B113-1)&amp;" "&amp;C113</f>
-        <v>F 13</v>
+        <v>F 9</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+      <c r="A114" t="s">
         <v>104</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114">
         <v>8</v>
       </c>
-      <c r="C114" s="1">
-        <v>18</v>
+      <c r="C114">
+        <v>14</v>
       </c>
       <c r="D114" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B114-1)&amp;" "&amp;C114</f>
-        <v>H 18</v>
+        <v>H 14</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+      <c r="A115" t="s">
         <v>7</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115">
         <v>13</v>
       </c>
-      <c r="C115" s="1">
-        <v>18</v>
+      <c r="C115">
+        <v>15</v>
       </c>
       <c r="D115" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B115-1)&amp;" "&amp;C115</f>
-        <v>M 18</v>
+        <v>M 15</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="A116" t="s">
         <v>41</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116">
         <v>10</v>
       </c>
-      <c r="C116" s="1">
-        <v>7</v>
+      <c r="C116">
+        <v>3</v>
       </c>
       <c r="D116" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B116-1)&amp;" "&amp;C116</f>
-        <v>J 7</v>
+        <v>J 3</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+      <c r="A117" t="s">
         <v>81</v>
       </c>
-      <c r="B117" s="1">
+      <c r="B117">
         <v>5</v>
       </c>
-      <c r="C117" s="1">
-        <v>14</v>
+      <c r="C117">
+        <v>10</v>
       </c>
       <c r="D117" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B117-1)&amp;" "&amp;C117</f>
-        <v>E 14</v>
+        <v>E 10</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="A118" t="s">
         <v>65</v>
       </c>
-      <c r="B118" s="1">
+      <c r="B118">
         <v>13</v>
       </c>
-      <c r="C118" s="1">
-        <v>9</v>
+      <c r="C118">
+        <v>6</v>
       </c>
       <c r="D118" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B118-1)&amp;" "&amp;C118</f>
-        <v>M 9</v>
+        <v>M 6</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+      <c r="A119" t="s">
         <v>107</v>
       </c>
-      <c r="B119" s="1">
+      <c r="B119">
         <v>15</v>
       </c>
-      <c r="C119" s="1">
-        <v>18</v>
+      <c r="C119">
+        <v>15</v>
       </c>
       <c r="D119" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B119-1)&amp;" "&amp;C119</f>
-        <v>O 18</v>
+        <v>O 15</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+      <c r="A120" t="s">
         <v>57</v>
       </c>
-      <c r="B120" s="1">
+      <c r="B120">
         <v>2</v>
       </c>
-      <c r="C120" s="1">
-        <v>31</v>
+      <c r="C120">
+        <v>27</v>
       </c>
       <c r="D120" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B120-1)&amp;" "&amp;C120</f>
-        <v>B 31</v>
+        <v>B 27</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+      <c r="A121" t="s">
         <v>90</v>
       </c>
-      <c r="B121" s="1">
+      <c r="B121">
         <v>10</v>
       </c>
-      <c r="C121" s="1">
-        <v>18</v>
+      <c r="C121">
+        <v>14</v>
       </c>
       <c r="D121" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B121-1)&amp;" "&amp;C121</f>
-        <v>J 18</v>
+        <v>J 14</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+      <c r="A122" t="s">
         <v>8</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122">
         <v>5</v>
       </c>
-      <c r="C122" s="1">
-        <v>15</v>
+      <c r="C122">
+        <v>11</v>
       </c>
       <c r="D122" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B122-1)&amp;" "&amp;C122</f>
-        <v>E 15</v>
+        <v>E 11</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+      <c r="A123" t="s">
         <v>5</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123">
         <v>11</v>
       </c>
-      <c r="C123" s="1">
-        <v>7</v>
+      <c r="C123">
+        <v>3</v>
       </c>
       <c r="D123" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B123-1)&amp;" "&amp;C123</f>
-        <v>K 7</v>
+        <v>K 3</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+      <c r="A124" t="s">
         <v>53</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124">
         <v>15</v>
       </c>
-      <c r="C124" s="1">
-        <v>22</v>
+      <c r="C124">
+        <v>18</v>
       </c>
       <c r="D124" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B124-1)&amp;" "&amp;C124</f>
-        <v>O 22</v>
+        <v>O 18</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
+      <c r="A125" t="s">
         <v>21</v>
       </c>
-      <c r="B125" s="1">
+      <c r="B125">
         <v>7</v>
       </c>
-      <c r="C125" s="1">
-        <v>30</v>
+      <c r="C125">
+        <v>26</v>
       </c>
       <c r="D125" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B125-1)&amp;" "&amp;C125</f>
-        <v>G 30</v>
+        <v>G 26</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+      <c r="A126" t="s">
         <v>23</v>
       </c>
-      <c r="B126" s="1">
+      <c r="B126">
         <v>17</v>
       </c>
-      <c r="C126" s="1">
-        <v>28</v>
+      <c r="C126">
+        <v>24</v>
       </c>
       <c r="D126" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B126-1)&amp;" "&amp;C126</f>
-        <v>Q 28</v>
+        <v>Q 24</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+      <c r="A127" t="s">
         <v>60</v>
       </c>
-      <c r="B127" s="1">
+      <c r="B127">
         <v>3</v>
       </c>
-      <c r="C127" s="1">
-        <v>16</v>
+      <c r="C127">
+        <v>12</v>
       </c>
       <c r="D127" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B127-1)&amp;" "&amp;C127</f>
-        <v>C 16</v>
+        <v>C 12</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+      <c r="A128" t="s">
         <v>112</v>
       </c>
-      <c r="B128" s="1">
+      <c r="B128">
         <v>26</v>
       </c>
-      <c r="C128" s="1">
-        <v>23</v>
+      <c r="C128">
+        <v>19</v>
       </c>
       <c r="D128" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B128-1)&amp;" "&amp;C128</f>
-        <v>Z 23</v>
+        <v>Z 19</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+      <c r="A129" t="s">
         <v>82</v>
       </c>
-      <c r="B129" s="1">
+      <c r="B129">
         <v>3</v>
       </c>
-      <c r="C129" s="1">
-        <v>12</v>
+      <c r="C129">
+        <v>8</v>
       </c>
       <c r="D129" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B129-1)&amp;" "&amp;C129</f>
-        <v>C 12</v>
+        <v>C 8</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+      <c r="A130" t="s">
         <v>59</v>
       </c>
-      <c r="B130" s="1">
+      <c r="B130">
         <v>15</v>
       </c>
-      <c r="C130" s="1">
-        <v>30</v>
+      <c r="C130">
+        <v>26</v>
       </c>
       <c r="D130" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B130-1)&amp;" "&amp;C130</f>
-        <v>O 30</v>
+        <v>O 26</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+      <c r="A131" t="s">
         <v>114</v>
       </c>
-      <c r="B131" s="1">
+      <c r="B131">
         <v>15</v>
       </c>
-      <c r="C131" s="1">
-        <v>23</v>
+      <c r="C131">
+        <v>19</v>
       </c>
       <c r="D131" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B131-1)&amp;" "&amp;C131</f>
-        <v>O 23</v>
+        <v>O 19</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+      <c r="A132" t="s">
         <v>124</v>
       </c>
-      <c r="B132" s="1">
+      <c r="B132">
         <v>26</v>
       </c>
-      <c r="C132" s="1">
-        <v>40</v>
+      <c r="C132">
+        <v>36</v>
       </c>
       <c r="D132" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B132-1)&amp;" "&amp;C132</f>
-        <v>Z 40</v>
+        <v>Z 36</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+      <c r="A133" t="s">
         <v>71</v>
       </c>
-      <c r="B133" s="1">
+      <c r="B133">
         <v>13</v>
       </c>
-      <c r="C133" s="1">
-        <v>26</v>
+      <c r="C133">
+        <v>22</v>
       </c>
       <c r="D133" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B133-1)&amp;" "&amp;C133</f>
-        <v>M 26</v>
+        <v>M 22</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
+      <c r="A134" t="s">
         <v>77</v>
       </c>
-      <c r="B134" s="1">
+      <c r="B134">
         <v>6</v>
       </c>
-      <c r="C134" s="1">
-        <v>20</v>
+      <c r="C134">
+        <v>16</v>
       </c>
       <c r="D134" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B134-1)&amp;" "&amp;C134</f>
-        <v>F 20</v>
+        <v>F 16</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+      <c r="A135" t="s">
         <v>52</v>
       </c>
-      <c r="B135" s="1">
+      <c r="B135">
         <v>12</v>
       </c>
-      <c r="C135" s="1">
-        <v>6</v>
+      <c r="C135">
+        <v>2</v>
       </c>
       <c r="D135" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B135-1)&amp;" "&amp;C135</f>
-        <v>L 6</v>
+        <v>L 2</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
+      <c r="A136" t="s">
         <v>27</v>
       </c>
-      <c r="B136" s="1">
+      <c r="B136">
         <v>25</v>
       </c>
-      <c r="C136" s="1">
-        <v>35</v>
+      <c r="C136">
+        <v>31</v>
       </c>
       <c r="D136" s="1" t="str">
         <f>CHAR(_xlfn.UNICODE("A") +B136-1)&amp;" "&amp;C136</f>
-        <v>Y 35</v>
+        <v>Y 31</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D136" xr:uid="{BFA92402-F1CC-4315-AAA9-B405F4265C28}"/>
   <sortState ref="A2:D136">
-    <sortCondition ref="A1"/>
+    <sortCondition ref="A2:A136"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3361,10 +3360,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -3387,7 +3386,7 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>LocatorListing!D2</f>
-        <v>I 24</v>
+        <v>I 20</v>
       </c>
       <c r="D1" s="1" t="str">
         <f>LocatorListing!A49</f>
@@ -3395,7 +3394,7 @@
       </c>
       <c r="E1" s="3" t="str">
         <f>LocatorListing!D49</f>
-        <v>M 10</v>
+        <v>M 6</v>
       </c>
       <c r="G1" s="1" t="str">
         <f>LocatorListing!A96</f>
@@ -3403,7 +3402,7 @@
       </c>
       <c r="H1" s="3" t="str">
         <f>LocatorListing!D96</f>
-        <v>U 25</v>
+        <v>U 21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3413,7 +3412,7 @@
       </c>
       <c r="B2" s="3" t="str">
         <f>LocatorListing!D3</f>
-        <v>I 28</v>
+        <v>I 24</v>
       </c>
       <c r="D2" s="1" t="str">
         <f>LocatorListing!A50</f>
@@ -3421,7 +3420,7 @@
       </c>
       <c r="E2" s="3" t="str">
         <f>LocatorListing!D50</f>
-        <v>Z 31</v>
+        <v>Y 27</v>
       </c>
       <c r="G2" s="1" t="str">
         <f>LocatorListing!A97</f>
@@ -3429,7 +3428,7 @@
       </c>
       <c r="H2" s="3" t="str">
         <f>LocatorListing!D97</f>
-        <v>M 7</v>
+        <v>M 3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3439,7 +3438,7 @@
       </c>
       <c r="B3" s="3" t="str">
         <f>LocatorListing!D4</f>
-        <v>B 25</v>
+        <v>B 21</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>LocatorListing!A51</f>
@@ -3447,7 +3446,7 @@
       </c>
       <c r="E3" s="3" t="str">
         <f>LocatorListing!D51</f>
-        <v>F 15</v>
+        <v>F 11</v>
       </c>
       <c r="G3" s="1" t="str">
         <f>LocatorListing!A98</f>
@@ -3455,7 +3454,7 @@
       </c>
       <c r="H3" s="3" t="str">
         <f>LocatorListing!D98</f>
-        <v>M 22</v>
+        <v>M 18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3465,7 +3464,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>LocatorListing!D5</f>
-        <v>X 22</v>
+        <v>X 18</v>
       </c>
       <c r="D4" s="1" t="str">
         <f>LocatorListing!A52</f>
@@ -3473,7 +3472,7 @@
       </c>
       <c r="E4" s="3" t="str">
         <f>LocatorListing!D52</f>
-        <v>B 27</v>
+        <v>B 23</v>
       </c>
       <c r="G4" s="1" t="str">
         <f>LocatorListing!A99</f>
@@ -3481,7 +3480,7 @@
       </c>
       <c r="H4" s="3" t="str">
         <f>LocatorListing!D99</f>
-        <v>C 23</v>
+        <v>C 19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3491,7 +3490,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>LocatorListing!D6</f>
-        <v>N 16</v>
+        <v>N 12</v>
       </c>
       <c r="D5" s="1" t="str">
         <f>LocatorListing!A53</f>
@@ -3499,7 +3498,7 @@
       </c>
       <c r="E5" s="3" t="str">
         <f>LocatorListing!D53</f>
-        <v>Q 29</v>
+        <v>Q 25</v>
       </c>
       <c r="G5" s="1" t="str">
         <f>LocatorListing!A100</f>
@@ -3507,7 +3506,7 @@
       </c>
       <c r="H5" s="3" t="str">
         <f>LocatorListing!D100</f>
-        <v>M 8</v>
+        <v>M 4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3517,7 +3516,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>LocatorListing!D7</f>
-        <v>G 23</v>
+        <v>G 20</v>
       </c>
       <c r="D6" s="1" t="str">
         <f>LocatorListing!A54</f>
@@ -3525,7 +3524,7 @@
       </c>
       <c r="E6" s="3" t="str">
         <f>LocatorListing!D54</f>
-        <v>U 32</v>
+        <v>U 28</v>
       </c>
       <c r="G6" s="1" t="str">
         <f>LocatorListing!A101</f>
@@ -3533,7 +3532,7 @@
       </c>
       <c r="H6" s="3" t="str">
         <f>LocatorListing!D101</f>
-        <v>Q 20</v>
+        <v>Q 16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3543,7 +3542,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f>LocatorListing!D8</f>
-        <v>N 12</v>
+        <v>N 8</v>
       </c>
       <c r="D7" s="1" t="str">
         <f>LocatorListing!A55</f>
@@ -3551,7 +3550,7 @@
       </c>
       <c r="E7" s="3" t="str">
         <f>LocatorListing!D55</f>
-        <v>N 24</v>
+        <v>N 20</v>
       </c>
       <c r="G7" s="1" t="str">
         <f>LocatorListing!A102</f>
@@ -3559,7 +3558,7 @@
       </c>
       <c r="H7" s="3" t="str">
         <f>LocatorListing!D102</f>
-        <v>B 15</v>
+        <v>B 12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3569,7 +3568,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f>LocatorListing!D9</f>
-        <v>G 19</v>
+        <v>G 15</v>
       </c>
       <c r="D8" s="1" t="str">
         <f>LocatorListing!A56</f>
@@ -3577,7 +3576,7 @@
       </c>
       <c r="E8" s="3" t="str">
         <f>LocatorListing!D56</f>
-        <v>N 20</v>
+        <v>N 16</v>
       </c>
       <c r="G8" s="1" t="str">
         <f>LocatorListing!A103</f>
@@ -3585,7 +3584,7 @@
       </c>
       <c r="H8" s="3" t="str">
         <f>LocatorListing!D103</f>
-        <v>R 22</v>
+        <v>R 18</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3595,7 +3594,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>LocatorListing!D10</f>
-        <v>C 11</v>
+        <v>C 7</v>
       </c>
       <c r="D9" s="1" t="str">
         <f>LocatorListing!A57</f>
@@ -3603,7 +3602,7 @@
       </c>
       <c r="E9" s="3" t="str">
         <f>LocatorListing!D57</f>
-        <v>H 33</v>
+        <v>H 29</v>
       </c>
       <c r="G9" s="1" t="str">
         <f>LocatorListing!A104</f>
@@ -3611,7 +3610,7 @@
       </c>
       <c r="H9" s="3" t="str">
         <f>LocatorListing!D104</f>
-        <v>I 6</v>
+        <v>I 2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3621,7 +3620,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f>LocatorListing!D11</f>
-        <v>Y 29</v>
+        <v>Y 26</v>
       </c>
       <c r="D10" s="1" t="str">
         <f>LocatorListing!A58</f>
@@ -3629,7 +3628,7 @@
       </c>
       <c r="E10" s="3" t="str">
         <f>LocatorListing!D58</f>
-        <v>G 24</v>
+        <v>G 20</v>
       </c>
       <c r="G10" s="1" t="str">
         <f>LocatorListing!A105</f>
@@ -3637,7 +3636,7 @@
       </c>
       <c r="H10" s="3" t="str">
         <f>LocatorListing!D105</f>
-        <v>E 11</v>
+        <v>E 7</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3647,7 +3646,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f>LocatorListing!D12</f>
-        <v>E 10</v>
+        <v>E 6</v>
       </c>
       <c r="D11" s="1" t="str">
         <f>LocatorListing!A59</f>
@@ -3655,7 +3654,7 @@
       </c>
       <c r="E11" s="3" t="str">
         <f>LocatorListing!D59</f>
-        <v>M 14</v>
+        <v>M 10</v>
       </c>
       <c r="G11" s="1" t="str">
         <f>LocatorListing!A106</f>
@@ -3663,7 +3662,7 @@
       </c>
       <c r="H11" s="3" t="str">
         <f>LocatorListing!D106</f>
-        <v>U 14</v>
+        <v>T 4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3673,7 +3672,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>LocatorListing!D13</f>
-        <v>R 26</v>
+        <v>R 22</v>
       </c>
       <c r="D12" s="1" t="str">
         <f>LocatorListing!A60</f>
@@ -3681,7 +3680,7 @@
       </c>
       <c r="E12" s="3" t="str">
         <f>LocatorListing!D60</f>
-        <v>B 11</v>
+        <v>B 7</v>
       </c>
       <c r="G12" s="1" t="str">
         <f>LocatorListing!A107</f>
@@ -3689,7 +3688,7 @@
       </c>
       <c r="H12" s="3" t="str">
         <f>LocatorListing!D107</f>
-        <v>R 40</v>
+        <v>R 36</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3699,7 +3698,7 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>LocatorListing!D14</f>
-        <v>C 20</v>
+        <v>C 16</v>
       </c>
       <c r="D13" s="1" t="str">
         <f>LocatorListing!A61</f>
@@ -3707,7 +3706,7 @@
       </c>
       <c r="E13" s="3" t="str">
         <f>LocatorListing!D61</f>
-        <v>C 15</v>
+        <v>C 11</v>
       </c>
       <c r="G13" s="1" t="str">
         <f>LocatorListing!A108</f>
@@ -3715,7 +3714,7 @@
       </c>
       <c r="H13" s="3" t="str">
         <f>LocatorListing!D108</f>
-        <v>G 29</v>
+        <v>G 25</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -3725,7 +3724,7 @@
       </c>
       <c r="B14" s="3" t="str">
         <f>LocatorListing!D15</f>
-        <v>S 24</v>
+        <v>S 20</v>
       </c>
       <c r="D14" s="1" t="str">
         <f>LocatorListing!A62</f>
@@ -3733,7 +3732,7 @@
       </c>
       <c r="E14" s="3" t="str">
         <f>LocatorListing!D62</f>
-        <v>U 28</v>
+        <v>U 24</v>
       </c>
       <c r="G14" s="1" t="str">
         <f>LocatorListing!A109</f>
@@ -3741,7 +3740,7 @@
       </c>
       <c r="H14" s="3" t="str">
         <f>LocatorListing!D109</f>
-        <v>O 8</v>
+        <v>O 4</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -3751,7 +3750,7 @@
       </c>
       <c r="B15" s="3" t="str">
         <f>LocatorListing!D16</f>
-        <v>J 28</v>
+        <v>J 24</v>
       </c>
       <c r="D15" s="1" t="str">
         <f>LocatorListing!A63</f>
@@ -3759,7 +3758,7 @@
       </c>
       <c r="E15" s="3" t="str">
         <f>LocatorListing!D63</f>
-        <v>F 34</v>
+        <v>F 30</v>
       </c>
       <c r="G15" s="1" t="str">
         <f>LocatorListing!A110</f>
@@ -3767,7 +3766,7 @@
       </c>
       <c r="H15" s="3" t="str">
         <f>LocatorListing!D110</f>
-        <v>M 30</v>
+        <v>M 27</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -3777,7 +3776,7 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>LocatorListing!D17</f>
-        <v>S 20</v>
+        <v>S 16</v>
       </c>
       <c r="D16" s="1" t="str">
         <f>LocatorListing!A64</f>
@@ -3785,7 +3784,7 @@
       </c>
       <c r="E16" s="3" t="str">
         <f>LocatorListing!D64</f>
-        <v>S 21</v>
+        <v>S 17</v>
       </c>
       <c r="G16" s="1" t="str">
         <f>LocatorListing!A111</f>
@@ -3793,7 +3792,7 @@
       </c>
       <c r="H16" s="3" t="str">
         <f>LocatorListing!D111</f>
-        <v>J 23</v>
+        <v>J 19</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -3803,7 +3802,7 @@
       </c>
       <c r="B17" s="3" t="str">
         <f>LocatorListing!D18</f>
-        <v>N 20</v>
+        <v>N 16</v>
       </c>
       <c r="D17" s="1" t="str">
         <f>LocatorListing!A65</f>
@@ -3811,7 +3810,7 @@
       </c>
       <c r="E17" s="3" t="str">
         <f>LocatorListing!D65</f>
-        <v>D 9</v>
+        <v>D 5</v>
       </c>
       <c r="G17" s="1" t="str">
         <f>LocatorListing!A112</f>
@@ -3819,7 +3818,7 @@
       </c>
       <c r="H17" s="3" t="str">
         <f>LocatorListing!D112</f>
-        <v>U 24</v>
+        <v>U 20</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -3829,7 +3828,7 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>LocatorListing!D19</f>
-        <v>I 20</v>
+        <v>I 16</v>
       </c>
       <c r="D18" s="1" t="str">
         <f>LocatorListing!A66</f>
@@ -3837,7 +3836,7 @@
       </c>
       <c r="E18" s="3" t="str">
         <f>LocatorListing!D66</f>
-        <v>Q 24</v>
+        <v>Q 20</v>
       </c>
       <c r="G18" s="1" t="str">
         <f>LocatorListing!A113</f>
@@ -3845,7 +3844,7 @@
       </c>
       <c r="H18" s="3" t="str">
         <f>LocatorListing!D113</f>
-        <v>F 13</v>
+        <v>F 9</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -3855,7 +3854,7 @@
       </c>
       <c r="B19" s="3" t="str">
         <f>LocatorListing!D20</f>
-        <v>T 34</v>
+        <v>T 30</v>
       </c>
       <c r="D19" s="1" t="str">
         <f>LocatorListing!A67</f>
@@ -3863,7 +3862,7 @@
       </c>
       <c r="E19" s="3" t="str">
         <f>LocatorListing!D67</f>
-        <v>Y 37</v>
+        <v>Y 33</v>
       </c>
       <c r="G19" s="1" t="str">
         <f>LocatorListing!A114</f>
@@ -3871,7 +3870,7 @@
       </c>
       <c r="H19" s="3" t="str">
         <f>LocatorListing!D114</f>
-        <v>H 18</v>
+        <v>H 14</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3881,7 +3880,7 @@
       </c>
       <c r="B20" s="3" t="str">
         <f>LocatorListing!D21</f>
-        <v>Q 25</v>
+        <v>Q 21</v>
       </c>
       <c r="D20" s="1" t="str">
         <f>LocatorListing!A68</f>
@@ -3889,7 +3888,7 @@
       </c>
       <c r="E20" s="3" t="str">
         <f>LocatorListing!D68</f>
-        <v>E 16</v>
+        <v>E 12</v>
       </c>
       <c r="G20" s="1" t="str">
         <f>LocatorListing!A115</f>
@@ -3897,7 +3896,7 @@
       </c>
       <c r="H20" s="3" t="str">
         <f>LocatorListing!D115</f>
-        <v>M 18</v>
+        <v>M 15</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -3907,7 +3906,7 @@
       </c>
       <c r="B21" s="3" t="str">
         <f>LocatorListing!D22</f>
-        <v>Q 32</v>
+        <v>Q 28</v>
       </c>
       <c r="D21" s="1" t="str">
         <f>LocatorListing!A69</f>
@@ -3915,7 +3914,7 @@
       </c>
       <c r="E21" s="3" t="str">
         <f>LocatorListing!D69</f>
-        <v>Q 21</v>
+        <v>Q 17</v>
       </c>
       <c r="G21" s="1" t="str">
         <f>LocatorListing!A116</f>
@@ -3923,7 +3922,7 @@
       </c>
       <c r="H21" s="3" t="str">
         <f>LocatorListing!D116</f>
-        <v>J 7</v>
+        <v>J 3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -3933,7 +3932,7 @@
       </c>
       <c r="B22" s="3" t="str">
         <f>LocatorListing!D23</f>
-        <v>K 19</v>
+        <v>K 15</v>
       </c>
       <c r="D22" s="1" t="str">
         <f>LocatorListing!A70</f>
@@ -3941,7 +3940,7 @@
       </c>
       <c r="E22" s="3" t="str">
         <f>LocatorListing!D70</f>
-        <v>J 7</v>
+        <v>J 3</v>
       </c>
       <c r="G22" s="1" t="str">
         <f>LocatorListing!A117</f>
@@ -3949,7 +3948,7 @@
       </c>
       <c r="H22" s="3" t="str">
         <f>LocatorListing!D117</f>
-        <v>E 14</v>
+        <v>E 10</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -3959,7 +3958,7 @@
       </c>
       <c r="B23" s="3" t="str">
         <f>LocatorListing!D24</f>
-        <v>O 14</v>
+        <v>O 10</v>
       </c>
       <c r="D23" s="1" t="str">
         <f>LocatorListing!A71</f>
@@ -3967,7 +3966,7 @@
       </c>
       <c r="E23" s="3" t="str">
         <f>LocatorListing!D71</f>
-        <v>S 36</v>
+        <v>S 32</v>
       </c>
       <c r="G23" s="1" t="str">
         <f>LocatorListing!A118</f>
@@ -3975,7 +3974,7 @@
       </c>
       <c r="H23" s="3" t="str">
         <f>LocatorListing!D118</f>
-        <v>M 9</v>
+        <v>M 6</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3985,7 +3984,7 @@
       </c>
       <c r="B24" s="3" t="str">
         <f>LocatorListing!D25</f>
-        <v>M 14</v>
+        <v>M 10</v>
       </c>
       <c r="D24" s="1" t="str">
         <f>LocatorListing!A72</f>
@@ -3993,7 +3992,7 @@
       </c>
       <c r="E24" s="3" t="str">
         <f>LocatorListing!D72</f>
-        <v>S 32</v>
+        <v>S 28</v>
       </c>
       <c r="G24" s="1" t="str">
         <f>LocatorListing!A119</f>
@@ -4001,7 +4000,7 @@
       </c>
       <c r="H24" s="3" t="str">
         <f>LocatorListing!D119</f>
-        <v>O 18</v>
+        <v>O 15</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -4011,7 +4010,7 @@
       </c>
       <c r="B25" s="3" t="str">
         <f>LocatorListing!D26</f>
-        <v>E 9</v>
+        <v>E 5</v>
       </c>
       <c r="D25" s="1" t="str">
         <f>LocatorListing!A73</f>
@@ -4019,7 +4018,7 @@
       </c>
       <c r="E25" s="3" t="str">
         <f>LocatorListing!D73</f>
-        <v>O 18</v>
+        <v>O 14</v>
       </c>
       <c r="G25" s="1" t="str">
         <f>LocatorListing!A120</f>
@@ -4027,7 +4026,7 @@
       </c>
       <c r="H25" s="3" t="str">
         <f>LocatorListing!D120</f>
-        <v>B 31</v>
+        <v>B 27</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -4037,7 +4036,7 @@
       </c>
       <c r="B26" s="3" t="str">
         <f>LocatorListing!D27</f>
-        <v>Q 33</v>
+        <v>Q 29</v>
       </c>
       <c r="D26" s="1" t="str">
         <f>LocatorListing!A74</f>
@@ -4045,7 +4044,7 @@
       </c>
       <c r="E26" s="3" t="str">
         <f>LocatorListing!D74</f>
-        <v>E 16</v>
+        <v>E 12</v>
       </c>
       <c r="G26" s="1" t="str">
         <f>LocatorListing!A121</f>
@@ -4053,7 +4052,7 @@
       </c>
       <c r="H26" s="3" t="str">
         <f>LocatorListing!D121</f>
-        <v>J 18</v>
+        <v>J 14</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -4063,7 +4062,7 @@
       </c>
       <c r="B27" s="3" t="str">
         <f>LocatorListing!D28</f>
-        <v>J 22</v>
+        <v>J 18</v>
       </c>
       <c r="D27" s="1" t="str">
         <f>LocatorListing!A75</f>
@@ -4071,7 +4070,7 @@
       </c>
       <c r="E27" s="3" t="str">
         <f>LocatorListing!D75</f>
-        <v>T 40</v>
+        <v>T 36</v>
       </c>
       <c r="G27" s="1" t="str">
         <f>LocatorListing!A122</f>
@@ -4079,7 +4078,7 @@
       </c>
       <c r="H27" s="3" t="str">
         <f>LocatorListing!D122</f>
-        <v>E 15</v>
+        <v>E 11</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -4089,7 +4088,7 @@
       </c>
       <c r="B28" s="3" t="str">
         <f>LocatorListing!D29</f>
-        <v>D 28</v>
+        <v>D 24</v>
       </c>
       <c r="D28" s="1" t="str">
         <f>LocatorListing!A76</f>
@@ -4097,7 +4096,7 @@
       </c>
       <c r="E28" s="3" t="str">
         <f>LocatorListing!D76</f>
-        <v>G 22</v>
+        <v>G 18</v>
       </c>
       <c r="G28" s="1" t="str">
         <f>LocatorListing!A123</f>
@@ -4105,7 +4104,7 @@
       </c>
       <c r="H28" s="3" t="str">
         <f>LocatorListing!D123</f>
-        <v>K 7</v>
+        <v>K 3</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -4115,7 +4114,7 @@
       </c>
       <c r="B29" s="3" t="str">
         <f>LocatorListing!D30</f>
-        <v>U 29</v>
+        <v>U 25</v>
       </c>
       <c r="D29" s="1" t="str">
         <f>LocatorListing!A77</f>
@@ -4123,7 +4122,7 @@
       </c>
       <c r="E29" s="3" t="str">
         <f>LocatorListing!D77</f>
-        <v>N 36</v>
+        <v>N 32</v>
       </c>
       <c r="G29" s="1" t="str">
         <f>LocatorListing!A124</f>
@@ -4131,7 +4130,7 @@
       </c>
       <c r="H29" s="3" t="str">
         <f>LocatorListing!D124</f>
-        <v>O 22</v>
+        <v>O 18</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -4141,7 +4140,7 @@
       </c>
       <c r="B30" s="3" t="str">
         <f>LocatorListing!D31</f>
-        <v>H 28</v>
+        <v>H 25</v>
       </c>
       <c r="D30" s="1" t="str">
         <f>LocatorListing!A78</f>
@@ -4149,7 +4148,7 @@
       </c>
       <c r="E30" s="3" t="str">
         <f>LocatorListing!D78</f>
-        <v>C 14</v>
+        <v>C 10</v>
       </c>
       <c r="G30" s="1" t="str">
         <f>LocatorListing!A125</f>
@@ -4157,7 +4156,7 @@
       </c>
       <c r="H30" s="3" t="str">
         <f>LocatorListing!D125</f>
-        <v>G 30</v>
+        <v>G 26</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -4167,7 +4166,7 @@
       </c>
       <c r="B31" s="3" t="str">
         <f>LocatorListing!D32</f>
-        <v>M 18</v>
+        <v>M 14</v>
       </c>
       <c r="D31" s="1" t="str">
         <f>LocatorListing!A79</f>
@@ -4175,7 +4174,7 @@
       </c>
       <c r="E31" s="3" t="str">
         <f>LocatorListing!D79</f>
-        <v>N 8</v>
+        <v>N 4</v>
       </c>
       <c r="G31" s="1" t="str">
         <f>LocatorListing!A126</f>
@@ -4183,7 +4182,7 @@
       </c>
       <c r="H31" s="3" t="str">
         <f>LocatorListing!D126</f>
-        <v>Q 28</v>
+        <v>Q 24</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -4193,7 +4192,7 @@
       </c>
       <c r="B32" s="3" t="str">
         <f>LocatorListing!D33</f>
-        <v>A 29</v>
+        <v>A 25</v>
       </c>
       <c r="D32" s="1" t="str">
         <f>LocatorListing!A80</f>
@@ -4201,7 +4200,7 @@
       </c>
       <c r="E32" s="3" t="str">
         <f>LocatorListing!D80</f>
-        <v>C 10</v>
+        <v>C 6</v>
       </c>
       <c r="G32" s="1" t="str">
         <f>LocatorListing!A127</f>
@@ -4209,7 +4208,7 @@
       </c>
       <c r="H32" s="3" t="str">
         <f>LocatorListing!D127</f>
-        <v>C 16</v>
+        <v>C 12</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -4219,7 +4218,7 @@
       </c>
       <c r="B33" s="3" t="str">
         <f>LocatorListing!D34</f>
-        <v>O 7</v>
+        <v>O 3</v>
       </c>
       <c r="D33" s="1" t="str">
         <f>LocatorListing!A81</f>
@@ -4227,7 +4226,7 @@
       </c>
       <c r="E33" s="3" t="str">
         <f>LocatorListing!D81</f>
-        <v>T 30</v>
+        <v>T 26</v>
       </c>
       <c r="G33" s="1" t="str">
         <f>LocatorListing!A128</f>
@@ -4235,7 +4234,7 @@
       </c>
       <c r="H33" s="3" t="str">
         <f>LocatorListing!D128</f>
-        <v>Z 23</v>
+        <v>Z 19</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -4245,7 +4244,7 @@
       </c>
       <c r="B34" s="3" t="str">
         <f>LocatorListing!D35</f>
-        <v>H 23</v>
+        <v>H 19</v>
       </c>
       <c r="D34" s="1" t="str">
         <f>LocatorListing!A82</f>
@@ -4253,7 +4252,7 @@
       </c>
       <c r="E34" s="3" t="str">
         <f>LocatorListing!D82</f>
-        <v>S 33</v>
+        <v>S 29</v>
       </c>
       <c r="G34" s="1" t="str">
         <f>LocatorListing!A129</f>
@@ -4261,7 +4260,7 @@
       </c>
       <c r="H34" s="3" t="str">
         <f>LocatorListing!D129</f>
-        <v>C 12</v>
+        <v>C 8</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -4271,7 +4270,7 @@
       </c>
       <c r="B35" s="3" t="str">
         <f>LocatorListing!D36</f>
-        <v>H 34</v>
+        <v>H 30</v>
       </c>
       <c r="D35" s="1" t="str">
         <f>LocatorListing!A83</f>
@@ -4279,7 +4278,7 @@
       </c>
       <c r="E35" s="3" t="str">
         <f>LocatorListing!D83</f>
-        <v>N 24</v>
+        <v>N 20</v>
       </c>
       <c r="G35" s="1" t="str">
         <f>LocatorListing!A130</f>
@@ -4287,7 +4286,7 @@
       </c>
       <c r="H35" s="3" t="str">
         <f>LocatorListing!D130</f>
-        <v>O 30</v>
+        <v>O 26</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -4297,7 +4296,7 @@
       </c>
       <c r="B36" s="3" t="str">
         <f>LocatorListing!D37</f>
-        <v>C 9</v>
+        <v>C 5</v>
       </c>
       <c r="D36" s="1" t="str">
         <f>LocatorListing!A84</f>
@@ -4305,7 +4304,7 @@
       </c>
       <c r="E36" s="3" t="str">
         <f>LocatorListing!D84</f>
-        <v>O 13</v>
+        <v>O 10</v>
       </c>
       <c r="G36" s="1" t="str">
         <f>LocatorListing!A131</f>
@@ -4313,7 +4312,7 @@
       </c>
       <c r="H36" s="3" t="str">
         <f>LocatorListing!D131</f>
-        <v>O 23</v>
+        <v>O 19</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -4323,7 +4322,7 @@
       </c>
       <c r="B37" s="3" t="str">
         <f>LocatorListing!D38</f>
-        <v>F 21</v>
+        <v>F 17</v>
       </c>
       <c r="D37" s="1" t="str">
         <f>LocatorListing!A85</f>
@@ -4331,7 +4330,7 @@
       </c>
       <c r="E37" s="3" t="str">
         <f>LocatorListing!D85</f>
-        <v>Z 27</v>
+        <v>Z 23</v>
       </c>
       <c r="G37" s="1" t="str">
         <f>LocatorListing!A132</f>
@@ -4339,7 +4338,7 @@
       </c>
       <c r="H37" s="3" t="str">
         <f>LocatorListing!D132</f>
-        <v>Z 40</v>
+        <v>Z 36</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -4349,7 +4348,7 @@
       </c>
       <c r="B38" s="3" t="str">
         <f>LocatorListing!D39</f>
-        <v>O 26</v>
+        <v>O 22</v>
       </c>
       <c r="D38" s="1" t="str">
         <f>LocatorListing!A86</f>
@@ -4357,7 +4356,7 @@
       </c>
       <c r="E38" s="3" t="str">
         <f>LocatorListing!D86</f>
-        <v>O 38</v>
+        <v>O 34</v>
       </c>
       <c r="G38" s="1" t="str">
         <f>LocatorListing!A133</f>
@@ -4365,7 +4364,7 @@
       </c>
       <c r="H38" s="3" t="str">
         <f>LocatorListing!D133</f>
-        <v>M 26</v>
+        <v>M 22</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -4375,7 +4374,7 @@
       </c>
       <c r="B39" s="3" t="str">
         <f>LocatorListing!D40</f>
-        <v>S 29</v>
+        <v>S 25</v>
       </c>
       <c r="D39" s="1" t="str">
         <f>LocatorListing!A87</f>
@@ -4383,7 +4382,7 @@
       </c>
       <c r="E39" s="3" t="str">
         <f>LocatorListing!D87</f>
-        <v>M 23</v>
+        <v>M 19</v>
       </c>
       <c r="G39" s="1" t="str">
         <f>LocatorListing!A134</f>
@@ -4391,7 +4390,7 @@
       </c>
       <c r="H39" s="3" t="str">
         <f>LocatorListing!D134</f>
-        <v>F 20</v>
+        <v>F 16</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -4401,7 +4400,7 @@
       </c>
       <c r="B40" s="3" t="str">
         <f>LocatorListing!D41</f>
-        <v>N 40</v>
+        <v>N 36</v>
       </c>
       <c r="D40" s="1" t="str">
         <f>LocatorListing!A88</f>
@@ -4409,7 +4408,7 @@
       </c>
       <c r="E40" s="3" t="str">
         <f>LocatorListing!D88</f>
-        <v>Z 33</v>
+        <v>Z 29</v>
       </c>
       <c r="G40" s="1" t="str">
         <f>LocatorListing!A135</f>
@@ -4417,7 +4416,7 @@
       </c>
       <c r="H40" s="3" t="str">
         <f>LocatorListing!D135</f>
-        <v>L 6</v>
+        <v>L 2</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -4427,7 +4426,7 @@
       </c>
       <c r="B41" s="3" t="str">
         <f>LocatorListing!D42</f>
-        <v>M 26</v>
+        <v>M 23</v>
       </c>
       <c r="D41" s="1" t="str">
         <f>LocatorListing!A89</f>
@@ -4435,7 +4434,7 @@
       </c>
       <c r="E41" s="3" t="str">
         <f>LocatorListing!D89</f>
-        <v>Q 39</v>
+        <v>Q 35</v>
       </c>
       <c r="G41" s="1" t="str">
         <f>LocatorListing!A136</f>
@@ -4443,7 +4442,7 @@
       </c>
       <c r="H41" s="3" t="str">
         <f>LocatorListing!D136</f>
-        <v>Y 35</v>
+        <v>Y 31</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -4453,7 +4452,7 @@
       </c>
       <c r="B42" s="3" t="str">
         <f>LocatorListing!D43</f>
-        <v>R 30</v>
+        <v>R 27</v>
       </c>
       <c r="D42" s="1" t="str">
         <f>LocatorListing!A90</f>
@@ -4461,7 +4460,7 @@
       </c>
       <c r="E42" s="3" t="str">
         <f>LocatorListing!D90</f>
-        <v>B 13</v>
+        <v>B 9</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="3"/>
@@ -4473,7 +4472,7 @@
       </c>
       <c r="B43" s="3" t="str">
         <f>LocatorListing!D44</f>
-        <v>H 7</v>
+        <v>H 3</v>
       </c>
       <c r="D43" s="1" t="str">
         <f>LocatorListing!A91</f>
@@ -4481,7 +4480,7 @@
       </c>
       <c r="E43" s="3" t="str">
         <f>LocatorListing!D91</f>
-        <v>J 20</v>
+        <v>J 16</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="3"/>
@@ -4493,7 +4492,7 @@
       </c>
       <c r="B44" s="3" t="str">
         <f>LocatorListing!D45</f>
-        <v>I 31</v>
+        <v>I 27</v>
       </c>
       <c r="D44" s="1" t="str">
         <f>LocatorListing!A92</f>
@@ -4501,7 +4500,7 @@
       </c>
       <c r="E44" s="3" t="str">
         <f>LocatorListing!D92</f>
-        <v>E 12</v>
+        <v>E 8</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="3"/>
@@ -4513,7 +4512,7 @@
       </c>
       <c r="B45" s="3" t="str">
         <f>LocatorListing!D46</f>
-        <v>N 16</v>
+        <v>N 12</v>
       </c>
       <c r="D45" s="1" t="str">
         <f>LocatorListing!A93</f>
@@ -4521,7 +4520,7 @@
       </c>
       <c r="E45" s="3" t="str">
         <f>LocatorListing!D93</f>
-        <v>M 30</v>
+        <v>M 26</v>
       </c>
       <c r="G45" s="1"/>
       <c r="H45" s="3"/>
@@ -4533,7 +4532,7 @@
       </c>
       <c r="B46" s="3" t="str">
         <f>LocatorListing!D47</f>
-        <v>Z 25</v>
+        <v>Y 21</v>
       </c>
       <c r="D46" s="1" t="str">
         <f>LocatorListing!A94</f>
@@ -4541,7 +4540,7 @@
       </c>
       <c r="E46" s="3" t="str">
         <f>LocatorListing!D94</f>
-        <v>U 33</v>
+        <v>U 29</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="3"/>
@@ -4553,7 +4552,7 @@
       </c>
       <c r="B47" s="3" t="str">
         <f>LocatorListing!D48</f>
-        <v>U 40</v>
+        <v>U 36</v>
       </c>
       <c r="D47" s="1" t="str">
         <f>LocatorListing!A95</f>
@@ -4561,7 +4560,7 @@
       </c>
       <c r="E47" s="3" t="str">
         <f>LocatorListing!D95</f>
-        <v>H 20</v>
+        <v>H 16</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="3"/>

</xml_diff>